<commit_message>
Se agrega Valor abs a la diff de Eva's
</commit_message>
<xml_diff>
--- a/Simulación Reses.xlsx
+++ b/Simulación Reses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acdzapata\Documents\Nutresa\Modelación\Compras en Oportunidad\Reses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422F40C3-C7FD-431D-88C8-955CDC719D16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAC0EB8-344B-4048-A1B2-BFBB92E661C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="11040" activeTab="1" xr2:uid="{E22285B9-2D93-4CF0-8AE6-2BCF1D496281}"/>
   </bookViews>
@@ -264,11 +264,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -898,7 +898,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
@@ -954,7 +954,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" t="s">
         <v>8</v>
       </c>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{970410AB-36A8-4264-BAF1-B96C385D7367}">
   <dimension ref="A2:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1477,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="2">
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="11">
@@ -1539,28 +1539,28 @@
         <v>22</v>
       </c>
       <c r="B18" s="11">
-        <f>B17*30%</f>
-        <v>48417.025531914893</v>
+        <f>B17*27%</f>
+        <v>43575.322978723409</v>
       </c>
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="11">
         <f>B17-B18</f>
-        <v>112973.05957446809</v>
+        <v>117814.76212765957</v>
       </c>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="8">
         <f>B19/B10</f>
-        <v>6.0364979735222063E-2</v>
+        <v>6.2952050295303E-2</v>
       </c>
       <c r="D20" s="11"/>
     </row>
@@ -1575,22 +1575,22 @@
       <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="11">
         <f>B19-B21</f>
-        <v>-111606.94042553191</v>
+        <v>-106765.23787234043</v>
       </c>
       <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="11">
         <f>B10+B14+B15+B18+B16+B21</f>
-        <v>2985048.9404255319</v>
+        <v>2980207.2378723403</v>
       </c>
       <c r="D23" s="11"/>
     </row>
@@ -1600,17 +1600,17 @@
       </c>
       <c r="B24" s="11">
         <f>B23/B8</f>
-        <v>7981.4142792126522</v>
+        <v>7968.4685504608024</v>
       </c>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="8">
         <f>(B2-B24)/B2</f>
-        <v>-3.8840853730658882E-2</v>
+        <v>-3.7155870162801294E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>